<commit_message>
Slight change in logic
</commit_message>
<xml_diff>
--- a/output/sample.xlsx
+++ b/output/sample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="12">
   <si>
     <t>DOCNO-1</t>
   </si>
@@ -32,16 +32,16 @@
     <t>1</t>
   </si>
   <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>c</t>
   </si>
   <si>
     <t>3</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>d</t>
@@ -172,7 +172,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -268,54 +268,54 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -342,6 +342,32 @@
       </c>
       <c r="H6" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>